<commit_message>
Improved All-Weather Portfolio by using sentiments
#12 - Improved All-Weather Portfolio by using sentiments as trading signals. A “bullish” trading signal would be assumed when the short-term sentiment (sent12) is higher than the longer-term sentiment (sent26).
- Optimised parameters using GA for two different objectives (maximise returns and minimise volatility)
#13 - Updated stocks and sentiment files
</commit_message>
<xml_diff>
--- a/SystemCode/frontend/smartportfolioWeb/src/smartportfolioWeb/portfolio_details.xlsx
+++ b/SystemCode/frontend/smartportfolioWeb/src/smartportfolioWeb/portfolio_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Edmund\Documents\GitHub\roboadvisorSystem\SystemCode\frontend\smartportfolioWeb\src\smartportfolioWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29D809A-3432-4D45-9714-30AF16A773C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987A5DA6-1126-4707-8406-CF77667FE700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>name</t>
   </si>
@@ -96,18 +96,6 @@
     <t>Utilise Hierarchical Risk Parity (HRP) to get the optimum portfolio to minimise volatility based on universe of 11 SPDR sector ETFs</t>
   </si>
   <si>
-    <t>Sector-based MPT+AI (max sharpe)</t>
-  </si>
-  <si>
-    <t>MPT+AI</t>
-  </si>
-  <si>
-    <t>Utilise Modern Portfolio Theory (MPT) to get the optimum portfolio to maximise sharpe ratio based on universe of 11 SPDR sector ETFs. Modify allocation based on AI model</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -121,6 +109,27 @@
   </si>
   <si>
     <t>hrp</t>
+  </si>
+  <si>
+    <t>Ray Dalio All Weather</t>
+  </si>
+  <si>
+    <t>crb</t>
+  </si>
+  <si>
+    <t>ALL_WEATHER</t>
+  </si>
+  <si>
+    <t>CRB</t>
+  </si>
+  <si>
+    <t>This simplified all-weather portfolio, by Ray Dalio, involves a mix of 30% stocks, 40% long-term U.S. bonds, 15% intermediate U.S. bonds, 7.5% gold and 7.5% other commodities. It is resilient enough to weather different "economic seasons". See https://kristal.ai/blog/all-weather-portfolio-kristals/ for more details</t>
+  </si>
+  <si>
+    <t>CRB+SENT</t>
+  </si>
+  <si>
+    <t>This is a modification of Ray Dalio's all-weather portfolio, that uses Twitter Sentiments as trading signals. Tweets are converted to Sentiments using a BERT model and then scaled for each stock component through optimisation with Genetic Algorithm</t>
   </si>
 </sst>
 </file>
@@ -450,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,7 +477,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -483,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -522,7 +531,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -561,7 +570,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
@@ -600,7 +609,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -621,43 +630,82 @@
         <v>24.15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>mpt+ai_spdr_max_sharpe</v>
+        <v>crb_all_weather_crb</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H5">
-        <v>-5.1100000000000003</v>
+        <v>-3.87</v>
       </c>
       <c r="I5">
-        <v>-2.1</v>
+        <v>2.44</v>
       </c>
       <c r="J5">
-        <v>11.12</v>
+        <v>14.33</v>
       </c>
       <c r="K5">
-        <v>4.1100000000000003</v>
+        <v>13.29</v>
       </c>
       <c r="L5">
-        <v>21.3</v>
+        <v>20.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f t="shared" ref="A6" si="1">LOWER(D6&amp;"_"&amp;E6&amp;"_"&amp;F6)</f>
+        <v>crb+sent_all_weather_crb</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>8.44</v>
+      </c>
+      <c r="I6">
+        <v>5.34</v>
+      </c>
+      <c r="J6">
+        <v>20.12</v>
+      </c>
+      <c r="K6">
+        <v>15.22</v>
+      </c>
+      <c r="L6">
+        <v>22.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>